<commit_message>
T1: Refactored and repaired 57, 100; T2: I Think that finished 29, only to assume and refactore
</commit_message>
<xml_diff>
--- a/Fizyka_Sprawka/Lab1_Cw100/FinalPrinted - Repaired.xlsx
+++ b/Fizyka_Sprawka/Lab1_Cw100/FinalPrinted - Repaired.xlsx
@@ -322,9 +322,9 @@
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.0000000000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1119,6 +1119,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1188,6 +1239,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1228,9 +1282,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1328,57 +1379,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -23857,9 +23857,9 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>31889</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4191725" cy="318036"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="4341766" cy="318036"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -23867,8 +23867,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="1746389"/>
-              <a:ext cx="4191725" cy="318036"/>
+              <a:off x="0" y="1772665"/>
+              <a:ext cx="4341766" cy="318036"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -24241,6 +24241,18 @@
                       </m:sSupPr>
                       <m:e>
                         <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>.00</m:t>
+                        </m:r>
+                        <m:r>
                           <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
@@ -24288,7 +24300,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -24296,8 +24308,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="1746389"/>
-              <a:ext cx="4191725" cy="318036"/>
+              <a:off x="0" y="1772665"/>
+              <a:ext cx="4341766" cy="318036"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -24377,7 +24389,31 @@
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>≈285〖𝑚𝑚〗^3</a:t>
+                <a:t>≈285〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>.00</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑚𝑚〗^3</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
@@ -37136,7 +37172,7 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>152309</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4037708" cy="265907"/>
+    <xdr:ext cx="4565994" cy="265907"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -37147,7 +37183,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="404996" y="1515117"/>
-              <a:ext cx="4037708" cy="265907"/>
+              <a:ext cx="4565994" cy="265907"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -37337,9 +37373,24 @@
                     </a:rPr>
                     <m:t>0.0058</m:t>
                   </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>≈</m:t>
+                  </m:r>
                 </m:oMath>
               </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> 0.006 </a:t>
+              </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -37353,7 +37404,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="404996" y="1515117"/>
-              <a:ext cx="4037708" cy="265907"/>
+              <a:ext cx="4565994" cy="265907"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -37380,7 +37431,6 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -37412,6 +37462,12 @@
                 <a:t> </a:t>
               </a:r>
               <a:r>
+                <a:rPr lang="en-US" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
@@ -37421,7 +37477,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>" /</a:t>
+                <a:t>/</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -37433,33 +37489,15 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>"</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>1425</a:t>
+                <a:t>"1425</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" i="0"/>
                 <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="el-GR" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                <a:rPr lang="en-US" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>" </a:t>
               </a:r>
@@ -37517,7 +37555,22 @@
                 </a:rPr>
                 <a:t>0.0058</a:t>
               </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>≈</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> 0.006 </a:t>
+              </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -41212,8 +41265,8 @@
       <xdr:rowOff>189257</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="312842" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -41305,7 +41358,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -41943,8 +41996,8 @@
       <xdr:rowOff>198782</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="312842" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -42036,7 +42089,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -42113,8 +42166,8 @@
       <xdr:rowOff>16566</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1350065" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -42249,7 +42302,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -42350,8 +42403,8 @@
       <xdr:rowOff>16565</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1350065" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10"/>
@@ -42412,7 +42465,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -42426,7 +42479,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10"/>
@@ -42498,9 +42551,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>273327</xdr:colOff>
+      <xdr:colOff>161269</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>49695</xdr:rowOff>
+      <xdr:rowOff>38489</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1350065" cy="172227"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -42512,7 +42565,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2617305" y="2824369"/>
+              <a:off x="2492093" y="2851165"/>
               <a:ext cx="1350065" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -42565,7 +42618,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -42587,7 +42640,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2617305" y="2824369"/>
+              <a:off x="2492093" y="2851165"/>
               <a:ext cx="1350065" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -42634,7 +42687,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -42916,7 +42969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -42935,39 +42988,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="92"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="119"/>
       <c r="I1" s="31"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="88" t="s">
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -42976,77 +43029,77 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="87"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="114"/>
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
       <c r="K3" s="18"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="153">
+      <c r="B4" s="83">
         <v>0.72</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="94"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="121"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="89"/>
-      <c r="H4" s="98"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="125"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="154">
+      <c r="B5" s="84">
         <v>8.24</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="96"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="123"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="99" t="s">
+      <c r="F5" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="83"/>
-      <c r="H5" s="100"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="127"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="35"/>
-      <c r="C6" s="101">
+      <c r="C6" s="128">
         <v>0.01</v>
       </c>
-      <c r="D6" s="102"/>
+      <c r="D6" s="129"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="105"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="132"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="83" t="s">
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
@@ -43079,18 +43132,18 @@
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83" t="s">
+      <c r="B11" s="110"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -43109,10 +43162,10 @@
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="83"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
+      <c r="A14" s="110"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -43149,18 +43202,18 @@
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83" t="s">
+      <c r="B18" s="110"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
@@ -43193,8 +43246,8 @@
       <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="83"/>
-      <c r="B22" s="83"/>
+      <c r="A22" s="110"/>
+      <c r="B22" s="110"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -43203,10 +43256,10 @@
       <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
+      <c r="A23" s="110"/>
+      <c r="B23" s="110"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="110"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -43243,10 +43296,10 @@
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="83"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
+      <c r="A27" s="110"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -43330,40 +43383,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="114"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="142"/>
       <c r="G1" s="51"/>
       <c r="H1" s="51"/>
       <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115"/>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="117"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="145"/>
       <c r="G2" s="51"/>
       <c r="H2" s="51"/>
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="88" t="s">
+      <c r="B3" s="113"/>
+      <c r="C3" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -43378,11 +43431,11 @@
       <c r="C4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="86"/>
-      <c r="F4" s="87"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="114"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -43391,15 +43444,15 @@
       <c r="A5" s="61">
         <v>1</v>
       </c>
-      <c r="B5" s="167">
+      <c r="B5" s="97">
         <v>8.44</v>
       </c>
       <c r="C5" s="63"/>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="93"/>
-      <c r="F5" s="94"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="121"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -43408,15 +43461,15 @@
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="168">
+      <c r="B6" s="98">
         <v>8.44</v>
       </c>
       <c r="C6" s="64"/>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="95"/>
-      <c r="F6" s="96"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="123"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -43425,17 +43478,17 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="169">
+      <c r="B7" s="99">
         <v>8.0500000000000007</v>
       </c>
       <c r="C7" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="96"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="123"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -43444,15 +43497,15 @@
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="169">
+      <c r="B8" s="99">
         <v>8.17</v>
       </c>
       <c r="C8" s="65"/>
-      <c r="D8" s="118" t="s">
+      <c r="D8" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="118"/>
-      <c r="F8" s="119"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="147"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -43461,15 +43514,15 @@
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="170">
+      <c r="B9" s="100">
         <v>8.01</v>
       </c>
-      <c r="C9" s="120" t="s">
+      <c r="C9" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="98"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="125"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -43478,17 +43531,17 @@
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="170">
+      <c r="B10" s="100">
         <v>8.06</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="85" t="s">
+      <c r="D10" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="86"/>
-      <c r="F10" s="87"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="114"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -43497,15 +43550,15 @@
       <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="170">
+      <c r="B11" s="100">
         <v>8.02</v>
       </c>
       <c r="C11" s="63"/>
-      <c r="D11" s="93">
+      <c r="D11" s="120">
         <v>0.05</v>
       </c>
-      <c r="E11" s="93"/>
-      <c r="F11" s="94"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="121"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -43514,15 +43567,15 @@
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="170">
+      <c r="B12" s="100">
         <v>8.02</v>
       </c>
       <c r="C12" s="72"/>
-      <c r="D12" s="106">
+      <c r="D12" s="134">
         <v>8.1669999999999998</v>
       </c>
-      <c r="E12" s="107"/>
-      <c r="F12" s="108"/>
+      <c r="E12" s="135"/>
+      <c r="F12" s="136"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -43531,17 +43584,17 @@
       <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="170">
+      <c r="B13" s="100">
         <v>8.0500000000000007</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="85">
+      <c r="D13" s="112">
         <v>10</v>
       </c>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="114"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -43550,20 +43603,20 @@
       <c r="A14" s="7">
         <v>10</v>
       </c>
-      <c r="B14" s="171">
+      <c r="B14" s="101">
         <v>8.41</v>
       </c>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="98"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="125"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="60"/>
-      <c r="B15" s="172">
+      <c r="B15" s="102">
         <f>AVERAGE(B5:B14)</f>
         <v>8.166999999999998</v>
       </c>
@@ -43576,14 +43629,14 @@
       <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="109" t="s">
+      <c r="A16" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="110"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="111"/>
+      <c r="B16" s="138"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
+      <c r="F16" s="139"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -43611,14 +43664,14 @@
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="109" t="s">
+      <c r="A19" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="111"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="138"/>
+      <c r="F19" s="139"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -43646,14 +43699,14 @@
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="110"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="111"/>
+      <c r="B22" s="138"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="139"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -43778,10 +43831,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A19:F19"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D13:F13"/>
@@ -43795,6 +43844,10 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43806,7 +43859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F4" sqref="F4:F14"/>
     </sheetView>
   </sheetViews>
@@ -43823,26 +43876,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="148" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="123"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="150"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="148" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="123"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="150"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -43861,21 +43914,21 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="173">
+      <c r="B4" s="103">
         <v>34.15</v>
       </c>
       <c r="C4" s="39">
         <f>POWER(B4-34.17,2)</f>
         <v>4.0000000000012508E-4</v>
       </c>
-      <c r="D4" s="177">
+      <c r="D4" s="107">
         <v>12</v>
       </c>
       <c r="E4" s="38">
         <f>POWER(D4-D14,2)</f>
         <v>4.622499999999994E-2</v>
       </c>
-      <c r="F4" s="177">
+      <c r="F4" s="107">
         <v>15.18</v>
       </c>
       <c r="G4" s="40">
@@ -43887,21 +43940,21 @@
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="174">
+      <c r="B5" s="104">
         <v>34</v>
       </c>
       <c r="C5" s="3">
         <f>POWER(B5-34.17,2)</f>
         <v>2.8900000000000581E-2</v>
       </c>
-      <c r="D5" s="178">
+      <c r="D5" s="108">
         <v>11.95</v>
       </c>
       <c r="E5" s="19">
         <f>POWER(D5-D14,2)</f>
         <v>7.0225000000000301E-2</v>
       </c>
-      <c r="F5" s="166">
+      <c r="F5" s="96">
         <v>15.75</v>
       </c>
       <c r="G5" s="6">
@@ -43913,21 +43966,21 @@
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="175">
+      <c r="B6" s="105">
         <v>34.1</v>
       </c>
       <c r="C6" s="3">
         <f>POWER(B6-34.17,2)</f>
         <v>4.9000000000000397E-3</v>
       </c>
-      <c r="D6" s="179">
+      <c r="D6" s="109">
         <v>12</v>
       </c>
       <c r="E6" s="3">
         <f>POWER(D6-D14,2)</f>
         <v>4.622499999999994E-2</v>
       </c>
-      <c r="F6" s="166">
+      <c r="F6" s="96">
         <v>15.8</v>
       </c>
       <c r="G6" s="6">
@@ -43939,21 +43992,21 @@
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="175">
+      <c r="B7" s="105">
         <v>34.1</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ref="C7:C13" si="0">POWER(B7-34.17,2)</f>
         <v>4.9000000000000397E-3</v>
       </c>
-      <c r="D7" s="178">
+      <c r="D7" s="108">
         <v>12</v>
       </c>
       <c r="E7" s="3">
         <f>POWER(D7-D14,2)</f>
         <v>4.622499999999994E-2</v>
       </c>
-      <c r="F7" s="166">
+      <c r="F7" s="96">
         <v>15.85</v>
       </c>
       <c r="G7" s="41">
@@ -43965,21 +44018,21 @@
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="175">
+      <c r="B8" s="105">
         <v>34.1</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
         <v>4.9000000000000397E-3</v>
       </c>
-      <c r="D8" s="178">
+      <c r="D8" s="108">
         <v>12</v>
       </c>
       <c r="E8" s="3">
         <f>POWER(D8-D14,2)</f>
         <v>4.622499999999994E-2</v>
       </c>
-      <c r="F8" s="166">
+      <c r="F8" s="96">
         <v>15.8</v>
       </c>
       <c r="G8" s="6">
@@ -43991,21 +44044,21 @@
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="175">
+      <c r="B9" s="105">
         <v>34.450000000000003</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
         <v>7.8400000000000636E-2</v>
       </c>
-      <c r="D9" s="178">
+      <c r="D9" s="108">
         <v>12.75</v>
       </c>
       <c r="E9" s="19">
         <f>POWER(D9-D14,2)</f>
         <v>0.28622500000000017</v>
       </c>
-      <c r="F9" s="166">
+      <c r="F9" s="96">
         <v>16.100000000000001</v>
       </c>
       <c r="G9" s="6">
@@ -44017,21 +44070,21 @@
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="175">
+      <c r="B10" s="105">
         <v>34.200000000000003</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
         <v>9.0000000000006817E-4</v>
       </c>
-      <c r="D10" s="178">
+      <c r="D10" s="108">
         <v>12.9</v>
       </c>
       <c r="E10" s="19">
         <f>POWER(D10-D14,2)</f>
         <v>0.46922500000000067</v>
       </c>
-      <c r="F10" s="166">
+      <c r="F10" s="96">
         <v>16</v>
       </c>
       <c r="G10" s="6">
@@ -44043,21 +44096,21 @@
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="175">
+      <c r="B11" s="105">
         <v>34.200000000000003</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="0"/>
         <v>9.0000000000006817E-4</v>
       </c>
-      <c r="D11" s="178">
+      <c r="D11" s="108">
         <v>11.8</v>
       </c>
       <c r="E11" s="19">
         <f>POWER(D11-D14,2)</f>
         <v>0.1722249999999993</v>
       </c>
-      <c r="F11" s="166">
+      <c r="F11" s="96">
         <v>16</v>
       </c>
       <c r="G11" s="6">
@@ -44069,21 +44122,21 @@
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="175">
+      <c r="B12" s="105">
         <v>34.4</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
         <v>5.2899999999998559E-2</v>
       </c>
-      <c r="D12" s="178">
+      <c r="D12" s="108">
         <v>11.8</v>
       </c>
       <c r="E12" s="19">
         <f>POWER(D12-D14,2)</f>
         <v>0.1722249999999993</v>
       </c>
-      <c r="F12" s="166">
+      <c r="F12" s="96">
         <v>16</v>
       </c>
       <c r="G12" s="6">
@@ -44095,21 +44148,21 @@
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="176">
+      <c r="B13" s="106">
         <v>34</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="0"/>
         <v>2.8900000000000581E-2</v>
       </c>
-      <c r="D13" s="166">
+      <c r="D13" s="96">
         <v>12.95</v>
       </c>
       <c r="E13" s="4">
         <f>POWER(D13-D14,2)</f>
         <v>0.54022499999999918</v>
       </c>
-      <c r="F13" s="166">
+      <c r="F13" s="96">
         <v>16.100000000000001</v>
       </c>
       <c r="G13" s="6">
@@ -44119,17 +44172,17 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="176">
+      <c r="B14" s="106">
         <f>AVERAGE(B4:B13)</f>
         <v>34.169999999999995</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="166">
+      <c r="D14" s="96">
         <f>AVERAGE(D4:D13)</f>
         <v>12.215</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="166">
+      <c r="F14" s="96">
         <f>AVERAGE(F4:F13)</f>
         <v>15.858000000000001</v>
       </c>
@@ -44156,29 +44209,29 @@
       <c r="G15" s="62"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="110" t="s">
+      <c r="A16" s="138" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="110"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="124" t="s">
+      <c r="B16" s="138"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="124"/>
-      <c r="G16" s="124"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="110" t="s">
+      <c r="A17" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="110"/>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="124" t="s">
+      <c r="B17" s="138"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="151" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="124"/>
+      <c r="F17" s="151"/>
       <c r="G17" s="44" t="s">
         <v>19</v>
       </c>
@@ -44188,8 +44241,8 @@
       <c r="B18" s="25"/>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="125"/>
-      <c r="F18" s="126"/>
+      <c r="E18" s="152"/>
+      <c r="F18" s="153"/>
       <c r="G18" s="66">
         <v>0.05</v>
       </c>
@@ -44199,22 +44252,22 @@
       <c r="B19" s="25"/>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
-      <c r="E19" s="110" t="s">
+      <c r="E19" s="138" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="138"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="25"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
-      <c r="E20" s="110" t="s">
+      <c r="E20" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="110"/>
-      <c r="G20" s="110"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="138"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
@@ -44226,12 +44279,12 @@
       <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="110" t="s">
+      <c r="A22" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="110"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
+      <c r="B22" s="138"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
       <c r="G22" s="27"/>
@@ -44259,11 +44312,11 @@
       <c r="B25" s="25"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
-      <c r="E25" s="110" t="s">
+      <c r="E25" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="138"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
@@ -44284,12 +44337,12 @@
       <c r="G27" s="27"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="110" t="s">
+      <c r="A28" s="138" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="110"/>
-      <c r="C28" s="110"/>
-      <c r="D28" s="110"/>
+      <c r="B28" s="138"/>
+      <c r="C28" s="138"/>
+      <c r="D28" s="138"/>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
       <c r="G28" s="27"/>
@@ -44317,11 +44370,11 @@
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
-      <c r="E31" s="110" t="s">
+      <c r="E31" s="138" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="110"/>
-      <c r="G31" s="110"/>
+      <c r="F31" s="138"/>
+      <c r="G31" s="138"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
@@ -44333,33 +44386,33 @@
       <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="110" t="s">
+      <c r="A33" s="138" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="110"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="138"/>
+      <c r="D33" s="138"/>
       <c r="E33" s="43"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27"/>
       <c r="H33" s="42"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="110" t="s">
+      <c r="A34" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="110"/>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
+      <c r="B34" s="138"/>
+      <c r="C34" s="138"/>
+      <c r="D34" s="138"/>
       <c r="E34" s="43"/>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="110"/>
-      <c r="B35" s="110"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="110"/>
+      <c r="A35" s="138"/>
+      <c r="B35" s="138"/>
+      <c r="C35" s="138"/>
+      <c r="D35" s="138"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
@@ -44386,12 +44439,12 @@
       <c r="D38" s="27"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="110" t="s">
+      <c r="A39" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="110"/>
-      <c r="C39" s="110"/>
-      <c r="D39" s="110"/>
+      <c r="B39" s="138"/>
+      <c r="C39" s="138"/>
+      <c r="D39" s="138"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
@@ -44439,12 +44492,12 @@
       <c r="G44" s="12"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="110" t="s">
+      <c r="A45" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="110"/>
-      <c r="C45" s="110"/>
-      <c r="D45" s="110"/>
+      <c r="B45" s="138"/>
+      <c r="C45" s="138"/>
+      <c r="D45" s="138"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -44550,7 +44603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
@@ -44562,28 +44615,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="155" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="129"/>
+      <c r="B2" s="156"/>
       <c r="C2" s="67"/>
       <c r="D2" s="67"/>
       <c r="E2" s="67"/>
       <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="130"/>
-      <c r="B3" s="131"/>
+      <c r="A3" s="157"/>
+      <c r="B3" s="158"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
@@ -44614,10 +44667,10 @@
       <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="110"/>
+      <c r="B7" s="138"/>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -44656,11 +44709,11 @@
       <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="138" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="110"/>
-      <c r="C12" s="110"/>
+      <c r="B12" s="138"/>
+      <c r="C12" s="138"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
@@ -44827,7 +44880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -44854,10 +44907,10 @@
       <c r="G1" s="78"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="155" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="129"/>
+      <c r="B2" s="156"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -44867,8 +44920,8 @@
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="130"/>
-      <c r="B3" s="131"/>
+      <c r="A3" s="157"/>
+      <c r="B3" s="158"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
@@ -44970,12 +45023,12 @@
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="110"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="110"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="138"/>
       <c r="E11" s="43"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -45008,12 +45061,12 @@
       <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="110" t="s">
+      <c r="A14" s="138" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="110"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
+      <c r="B14" s="138"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
       <c r="E14" s="43"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -45022,14 +45075,14 @@
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="128" t="s">
+      <c r="A15" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="129"/>
-      <c r="C15" s="128" t="s">
+      <c r="B15" s="156"/>
+      <c r="C15" s="155" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="129"/>
+      <c r="D15" s="156"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -45037,10 +45090,10 @@
       <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="130"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="130"/>
-      <c r="D16" s="131"/>
+      <c r="A16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="157"/>
+      <c r="D16" s="158"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -45472,7 +45525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -45485,16 +45538,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="112" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="87"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="114"/>
       <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -45504,10 +45557,10 @@
       <c r="B2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="132" t="s">
+      <c r="C2" s="159" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="133"/>
+      <c r="D2" s="160"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -45521,8 +45574,8 @@
       <c r="B3" s="49">
         <v>0.72</v>
       </c>
-      <c r="C3" s="132"/>
-      <c r="D3" s="133"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
@@ -45536,8 +45589,8 @@
       <c r="B4" s="52">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="C4" s="132"/>
-      <c r="D4" s="133"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="160"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -45551,8 +45604,8 @@
       <c r="B5" s="73">
         <v>7.04</v>
       </c>
-      <c r="C5" s="132"/>
-      <c r="D5" s="133"/>
+      <c r="C5" s="159"/>
+      <c r="D5" s="160"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -45566,8 +45619,8 @@
       <c r="B6" s="79">
         <v>285</v>
       </c>
-      <c r="C6" s="134"/>
-      <c r="D6" s="135"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="162"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -45575,16 +45628,16 @@
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="138" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
       <c r="J7" s="80"/>
       <c r="K7" s="80"/>
     </row>
@@ -45609,16 +45662,16 @@
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="110" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
@@ -45827,7 +45880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -45841,15 +45894,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="112" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="87"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="55"/>
       <c r="I1" s="55"/>
     </row>
@@ -45860,10 +45913,10 @@
       <c r="B2" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="132" t="s">
+      <c r="C2" s="159" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="133"/>
+      <c r="D2" s="160"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="15"/>
@@ -45875,8 +45928,8 @@
       <c r="B3" s="12">
         <v>8.24</v>
       </c>
-      <c r="C3" s="132"/>
-      <c r="D3" s="133"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="15"/>
@@ -45888,8 +45941,8 @@
       <c r="B4" s="13">
         <v>1425</v>
       </c>
-      <c r="C4" s="132"/>
-      <c r="D4" s="133"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="160"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="15"/>
@@ -45901,8 +45954,8 @@
       <c r="B5" s="13">
         <v>75</v>
       </c>
-      <c r="C5" s="132"/>
-      <c r="D5" s="133"/>
+      <c r="C5" s="159"/>
+      <c r="D5" s="160"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="15"/>
@@ -45914,22 +45967,22 @@
       <c r="B6" s="13">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="C6" s="134"/>
-      <c r="D6" s="135"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="162"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="136" t="s">
+      <c r="A7" s="163" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="137"/>
-      <c r="C7" s="137"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="138"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="164"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="165"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
@@ -45959,15 +46012,15 @@
       <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="112" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="87"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="114"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
@@ -46072,7 +46125,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B14"/>
+      <selection activeCell="F33" sqref="F33:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46087,28 +46140,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="166" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="149" t="s">
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="176" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="152" t="s">
+      <c r="G1" s="179" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="142"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="133"/>
+      <c r="A2" s="169"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="160"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -46126,155 +46179,155 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="150"/>
-      <c r="G3" s="133"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="160"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="158">
+      <c r="B4" s="88">
         <v>8.44</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="150"/>
-      <c r="G4" s="133"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="160"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="159">
+      <c r="B5" s="89">
         <v>8.44</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="150"/>
-      <c r="G5" s="133"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="160"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="161">
+      <c r="B6" s="91">
         <v>8.0500000000000007</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="150"/>
-      <c r="G6" s="133"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="177"/>
+      <c r="G6" s="160"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="161">
+      <c r="B7" s="91">
         <v>8.17</v>
       </c>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="150"/>
-      <c r="G7" s="133"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="160"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="160">
+      <c r="B8" s="90">
         <v>8.01</v>
       </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="150"/>
-      <c r="G8" s="133"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="177"/>
+      <c r="G8" s="160"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="160">
+      <c r="B9" s="90">
         <v>8.06</v>
       </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="150"/>
-      <c r="G9" s="133"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="177"/>
+      <c r="G9" s="160"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="160">
+      <c r="B10" s="90">
         <v>8.02</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="150"/>
-      <c r="G10" s="133"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="177"/>
+      <c r="G10" s="160"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="160">
+      <c r="B11" s="90">
         <v>8.02</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="150"/>
-      <c r="G11" s="133"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="160"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="160">
+      <c r="B12" s="90">
         <v>8.0500000000000007</v>
       </c>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="150"/>
-      <c r="G12" s="133"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="177"/>
+      <c r="G12" s="160"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="161">
+      <c r="B13" s="91">
         <v>8.41</v>
       </c>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="133"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="160"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="161">
+      <c r="B14" s="91">
         <v>8.1669999999999998</v>
       </c>
-      <c r="C14" s="155">
+      <c r="C14" s="85">
         <v>0.72</v>
       </c>
-      <c r="D14" s="156">
+      <c r="D14" s="86">
         <v>285</v>
       </c>
-      <c r="E14" s="157">
+      <c r="E14" s="87">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="F14" s="150"/>
-      <c r="G14" s="133"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="160"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -46284,10 +46337,10 @@
       <c r="C15" s="4">
         <v>0</v>
       </c>
-      <c r="D15" s="145"/>
-      <c r="E15" s="146"/>
-      <c r="F15" s="150"/>
-      <c r="G15" s="133"/>
+      <c r="D15" s="172"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="177"/>
+      <c r="G15" s="160"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -46297,10 +46350,10 @@
       <c r="C16" s="4">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D16" s="147"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="150"/>
-      <c r="G16" s="133"/>
+      <c r="D16" s="174"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="177"/>
+      <c r="G16" s="160"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -46316,39 +46369,39 @@
       <c r="E17" s="81">
         <v>6.5639E-5</v>
       </c>
-      <c r="F17" s="151"/>
-      <c r="G17" s="135"/>
+      <c r="F17" s="178"/>
+      <c r="G17" s="162"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="112" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="87"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="114"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="139" t="s">
+      <c r="A19" s="166" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="140"/>
-      <c r="C19" s="140"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="141"/>
+      <c r="B19" s="167"/>
+      <c r="C19" s="167"/>
+      <c r="D19" s="167"/>
+      <c r="E19" s="167"/>
+      <c r="F19" s="167"/>
+      <c r="G19" s="168"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="142"/>
-      <c r="B20" s="143"/>
-      <c r="C20" s="143"/>
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="G20" s="144"/>
+      <c r="A20" s="169"/>
+      <c r="B20" s="170"/>
+      <c r="C20" s="170"/>
+      <c r="D20" s="170"/>
+      <c r="E20" s="170"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="171"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -46377,194 +46430,194 @@
       <c r="A22" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="158">
+      <c r="B22" s="88">
         <v>34.15</v>
       </c>
-      <c r="C22" s="162">
+      <c r="C22" s="92">
         <v>12</v>
       </c>
-      <c r="D22" s="165">
+      <c r="D22" s="95">
         <v>15.18</v>
       </c>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="94"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
+      <c r="G22" s="121"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2</v>
       </c>
-      <c r="B23" s="159">
+      <c r="B23" s="89">
         <v>34</v>
       </c>
-      <c r="C23" s="163">
+      <c r="C23" s="93">
         <v>11.95</v>
       </c>
-      <c r="D23" s="166">
+      <c r="D23" s="96">
         <v>15.75</v>
       </c>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="96"/>
+      <c r="E23" s="122"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="123"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3</v>
       </c>
-      <c r="B24" s="160">
+      <c r="B24" s="90">
         <v>34.1</v>
       </c>
-      <c r="C24" s="155">
+      <c r="C24" s="85">
         <v>12</v>
       </c>
-      <c r="D24" s="166">
+      <c r="D24" s="96">
         <v>15.8</v>
       </c>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="96"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="123"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>4</v>
       </c>
-      <c r="B25" s="160">
+      <c r="B25" s="90">
         <v>34.1</v>
       </c>
-      <c r="C25" s="163">
+      <c r="C25" s="93">
         <v>12</v>
       </c>
-      <c r="D25" s="166">
+      <c r="D25" s="96">
         <v>15.85</v>
       </c>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="96"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="123"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>5</v>
       </c>
-      <c r="B26" s="160">
+      <c r="B26" s="90">
         <v>34.1</v>
       </c>
-      <c r="C26" s="163">
+      <c r="C26" s="93">
         <v>12</v>
       </c>
-      <c r="D26" s="166">
+      <c r="D26" s="96">
         <v>15.8</v>
       </c>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="96"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="123"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>6</v>
       </c>
-      <c r="B27" s="160">
+      <c r="B27" s="90">
         <v>34.450000000000003</v>
       </c>
-      <c r="C27" s="163">
+      <c r="C27" s="93">
         <v>12.75</v>
       </c>
-      <c r="D27" s="166">
+      <c r="D27" s="96">
         <v>16.100000000000001</v>
       </c>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="96"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="123"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>7</v>
       </c>
-      <c r="B28" s="160">
+      <c r="B28" s="90">
         <v>34.200000000000003</v>
       </c>
-      <c r="C28" s="163">
+      <c r="C28" s="93">
         <v>12.9</v>
       </c>
-      <c r="D28" s="166">
+      <c r="D28" s="96">
         <v>16</v>
       </c>
-      <c r="E28" s="95"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="96"/>
+      <c r="E28" s="122"/>
+      <c r="F28" s="122"/>
+      <c r="G28" s="123"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>8</v>
       </c>
-      <c r="B29" s="160">
+      <c r="B29" s="90">
         <v>34.200000000000003</v>
       </c>
-      <c r="C29" s="163">
+      <c r="C29" s="93">
         <v>11.8</v>
       </c>
-      <c r="D29" s="166">
+      <c r="D29" s="96">
         <v>16</v>
       </c>
-      <c r="E29" s="95"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="96"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="123"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>9</v>
       </c>
-      <c r="B30" s="160">
+      <c r="B30" s="90">
         <v>34.4</v>
       </c>
-      <c r="C30" s="163">
+      <c r="C30" s="93">
         <v>11.8</v>
       </c>
-      <c r="D30" s="166">
+      <c r="D30" s="96">
         <v>16</v>
       </c>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="96"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="122"/>
+      <c r="G30" s="123"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>10</v>
       </c>
-      <c r="B31" s="161">
+      <c r="B31" s="91">
         <v>34</v>
       </c>
-      <c r="C31" s="164">
+      <c r="C31" s="94">
         <v>12.95</v>
       </c>
-      <c r="D31" s="166">
+      <c r="D31" s="96">
         <v>16.100000000000001</v>
       </c>
-      <c r="E31" s="95"/>
-      <c r="F31" s="95"/>
-      <c r="G31" s="96"/>
+      <c r="E31" s="122"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="123"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="161">
+      <c r="B32" s="91">
         <f>AVERAGE(B22:B31)</f>
         <v>34.169999999999995</v>
       </c>
-      <c r="C32" s="164">
+      <c r="C32" s="94">
         <f>AVERAGE(C22:C31)</f>
         <v>12.215</v>
       </c>
-      <c r="D32" s="166">
+      <c r="D32" s="96">
         <f>AVERAGE(D22:D31)</f>
         <v>15.858000000000001</v>
       </c>
-      <c r="E32" s="155">
+      <c r="E32" s="85">
         <v>8.24</v>
       </c>
       <c r="F32" s="3">
         <v>1425</v>
       </c>
       <c r="G32" s="5">
-        <v>5.7999999999999996E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -46581,8 +46634,8 @@
       <c r="E33" s="19">
         <v>0</v>
       </c>
-      <c r="F33" s="95"/>
-      <c r="G33" s="96"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="123"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
@@ -46598,8 +46651,8 @@
       <c r="E34" s="19">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="F34" s="95"/>
-      <c r="G34" s="96"/>
+      <c r="F34" s="122"/>
+      <c r="G34" s="123"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
@@ -46623,15 +46676,15 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="112" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="87"/>
+      <c r="B36" s="113"/>
+      <c r="C36" s="113"/>
+      <c r="D36" s="113"/>
+      <c r="E36" s="113"/>
+      <c r="F36" s="113"/>
+      <c r="G36" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>